<commit_message>
small changes and bug fixes
</commit_message>
<xml_diff>
--- a/IO_CheckRules/RunControl_CheckRules.xlsx
+++ b/IO_CheckRules/RunControl_CheckRules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="213">
   <si>
     <t>Sheet #</t>
   </si>
@@ -566,22 +566,109 @@
     <t>ea_r</t>
   </si>
   <si>
-    <t>Simple Return, Active Only,  new hire.</t>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 20-20,  no new hire.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 30-30,  no new hire.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 50-50,  no new hire.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 60-60,  no new hire.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 40-40,  no new hire.</t>
   </si>
   <si>
     <t>R20</t>
   </si>
   <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
-    <t>R60</t>
+    <t>Simple Return, Active Only 60-60,  new hires.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 20-20,  new hires.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 30-30,  new hires.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 40-40,  new hires.</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 50-50,  new hires.</t>
+  </si>
+  <si>
+    <t>R20h</t>
+  </si>
+  <si>
+    <t>R30h</t>
+  </si>
+  <si>
+    <t>R40h</t>
+  </si>
+  <si>
+    <t>R50h</t>
+  </si>
+  <si>
+    <t>R60h</t>
+  </si>
+  <si>
+    <t>R20hs</t>
+  </si>
+  <si>
+    <t>R30hs</t>
+  </si>
+  <si>
+    <t>R40hs</t>
+  </si>
+  <si>
+    <t>R50hs</t>
+  </si>
+  <si>
+    <t>R60hs</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 20-20,  new hires. Stochastic Return</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 30-30,  new hires. Stochastic Return</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 40-40,  new hires. Stochastic Return</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 50-50,  new hires. Stochastic Return</t>
+  </si>
+  <si>
+    <t>Simple Return, Active Only 60-60,  new hires. Stochastic Return</t>
+  </si>
+  <si>
+    <t>R20hs2</t>
+  </si>
+  <si>
+    <t>R30hs2</t>
+  </si>
+  <si>
+    <t>R40hs2</t>
+  </si>
+  <si>
+    <t>R50hs2</t>
+  </si>
+  <si>
+    <t>R60hs2</t>
   </si>
 </sst>
 </file>
@@ -762,7 +849,13 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -771,16 +864,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1198,7 +1285,7 @@
   <dimension ref="A6:A25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,13 +1371,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ10"/>
+  <dimension ref="A1:AQ28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:A10"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,68 +1546,68 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="25" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="25" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="26" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="27" t="s">
+      <c r="Z4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="28" t="s">
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
       <c r="AG4" s="16"/>
       <c r="AH4" s="23"/>
       <c r="AI4" s="21"/>
-      <c r="AJ4" s="24" t="s">
+      <c r="AJ4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
       <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1662,13 +1749,12 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C6" s="11" t="b">
-        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -1794,13 +1880,13 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C7" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>109</v>
@@ -1896,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="2" t="s">
         <v>168</v>
@@ -1925,13 +2011,13 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C8" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>109</v>
@@ -2027,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="AI8" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="2" t="s">
         <v>168</v>
@@ -2056,13 +2142,13 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
@@ -2158,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="AI9" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9" s="2" t="s">
         <v>168</v>
@@ -2187,13 +2273,13 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>109</v>
@@ -2289,7 +2375,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10" s="2" t="s">
         <v>168</v>
@@ -2316,93 +2402,2058 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>65</v>
+      </c>
+      <c r="O12">
+        <v>65</v>
+      </c>
+      <c r="P12" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12">
+        <v>10</v>
+      </c>
+      <c r="S12" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T12" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U12" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W12" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X12" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB12">
+        <v>30</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD12" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE12" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF12" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK12" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <v>200</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN12">
+        <v>10</v>
+      </c>
+      <c r="AO12">
+        <v>200</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>65</v>
+      </c>
+      <c r="O13">
+        <v>65</v>
+      </c>
+      <c r="P13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U13" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W13" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB13">
+        <v>30</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD13" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE13" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF13" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK13" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>200</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN13">
+        <v>10</v>
+      </c>
+      <c r="AO13">
+        <v>200</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>65</v>
+      </c>
+      <c r="O14">
+        <v>65</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U14" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V14" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W14" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X14" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB14">
+        <v>30</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD14" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE14" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF14" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK14" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>200</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN14">
+        <v>10</v>
+      </c>
+      <c r="AO14">
+        <v>200</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" t="s">
+        <v>170</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>65</v>
+      </c>
+      <c r="O15">
+        <v>65</v>
+      </c>
+      <c r="P15" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T15" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U15" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V15" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W15" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB15">
+        <v>30</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD15" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE15" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF15" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK15" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL15">
+        <v>200</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN15">
+        <v>10</v>
+      </c>
+      <c r="AO15">
+        <v>200</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>65</v>
+      </c>
+      <c r="O16">
+        <v>65</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB16">
+        <v>30</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD16" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE16" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF16" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK16" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>200</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN16">
+        <v>10</v>
+      </c>
+      <c r="AO16">
+        <v>200</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="O18">
+        <v>65</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U18" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V18" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W18" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB18">
+        <v>30</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD18" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE18" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF18" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK18" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>200</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN18">
+        <v>10</v>
+      </c>
+      <c r="AO18">
+        <v>200</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>65</v>
+      </c>
+      <c r="O19">
+        <v>65</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U19" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W19" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB19">
+        <v>30</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD19" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE19" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF19" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK19" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>200</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN19">
+        <v>10</v>
+      </c>
+      <c r="AO19">
+        <v>200</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" t="s">
+        <v>170</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>65</v>
+      </c>
+      <c r="O20">
+        <v>65</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q20">
+        <v>10</v>
+      </c>
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T20" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U20" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V20" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W20" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB20">
+        <v>30</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD20" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE20" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF20" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK20" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL20">
+        <v>200</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN20">
+        <v>10</v>
+      </c>
+      <c r="AO20">
+        <v>200</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>65</v>
+      </c>
+      <c r="O21">
+        <v>65</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>10</v>
+      </c>
+      <c r="S21" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T21" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U21" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V21" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W21" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X21" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB21">
+        <v>30</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD21" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE21" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF21" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG21" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK21" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL21">
+        <v>200</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN21">
+        <v>10</v>
+      </c>
+      <c r="AO21">
+        <v>200</v>
+      </c>
+      <c r="AP21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>65</v>
+      </c>
+      <c r="O22">
+        <v>65</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q22">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="S22" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T22" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U22" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V22" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W22" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X22" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB22">
+        <v>30</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD22" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE22" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF22" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK22" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL22">
+        <v>200</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN22">
+        <v>10</v>
+      </c>
+      <c r="AO22">
+        <v>200</v>
+      </c>
+      <c r="AP22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" t="s">
+        <v>170</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>65</v>
+      </c>
+      <c r="O24">
+        <v>65</v>
+      </c>
+      <c r="P24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>10</v>
+      </c>
+      <c r="S24" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U24" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V24" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W24" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X24" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB24">
+        <v>30</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD24" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE24" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF24" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG24" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK24" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="AL24">
+        <v>200</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN24">
+        <v>10</v>
+      </c>
+      <c r="AO24">
+        <v>200</v>
+      </c>
+      <c r="AP24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" t="s">
+        <v>170</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>65</v>
+      </c>
+      <c r="O25">
+        <v>65</v>
+      </c>
+      <c r="P25" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q25">
+        <v>10</v>
+      </c>
+      <c r="R25">
+        <v>10</v>
+      </c>
+      <c r="S25" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T25" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U25" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V25" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W25" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X25" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB25">
+        <v>30</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD25" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE25" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF25" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG25" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK25" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="AL25">
+        <v>200</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN25">
+        <v>10</v>
+      </c>
+      <c r="AO25">
+        <v>200</v>
+      </c>
+      <c r="AP25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" t="s">
+        <v>147</v>
+      </c>
+      <c r="I26" t="s">
+        <v>170</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>65</v>
+      </c>
+      <c r="O26">
+        <v>65</v>
+      </c>
+      <c r="P26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="S26" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U26" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V26" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W26" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB26">
+        <v>30</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD26" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE26" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF26" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK26" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="AL26">
+        <v>200</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN26">
+        <v>10</v>
+      </c>
+      <c r="AO26">
+        <v>200</v>
+      </c>
+      <c r="AP26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>65</v>
+      </c>
+      <c r="O27">
+        <v>65</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V27" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X27" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB27">
+        <v>30</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD27" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE27" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF27" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG27" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK27" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="AL27">
+        <v>200</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN27">
+        <v>10</v>
+      </c>
+      <c r="AO27">
+        <v>200</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" t="s">
+        <v>170</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <v>65</v>
+      </c>
+      <c r="O28">
+        <v>65</v>
+      </c>
+      <c r="P28" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q28">
+        <v>10</v>
+      </c>
+      <c r="R28">
+        <v>10</v>
+      </c>
+      <c r="S28" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T28" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U28" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V28" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="W28" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X28" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB28">
+        <v>30</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD28" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AE28" s="13">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF28" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="AG28" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK28" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="AL28">
+        <v>200</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN28">
+        <v>10</v>
+      </c>
+      <c r="AO28">
+        <v>200</v>
+      </c>
+      <c r="AP28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ28">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP10 AP12:AP16 AP18:AP22 AP24:AP28">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA10 AA12:AA16 AA18:AA22 AA24:AA28">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z10 Z12:Z16 Z18:Z22 Z24:Z28">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC10 AC12:AC16 AC18:AC22 AC24:AC28">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C10 K6:K10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K10 C18:C22 K24:K28 K12:K16 C6:C10 K18:K22 C12:C16 C24:C28">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N10 N12:N16 N18:N22 N24:N28">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T10 P6:P10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T10 P6:P10 T12:T16 P12:P16 T18:T22 P18:P22 T24:T28 P24:P28">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R10 Q12:R16 Q18:R22 Q24:R28">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6:W10 S6:S10 U6:U10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6:W10 S6:S10 U6:U10 W12:W16 S12:S16 U12:U16 W18:W22 S18:S22 U18:U22 W24:W28 S24:S28 U24:U28">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB10 AB12:AB16 AB18:AB22 AB24:AB28">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE10 AD12:AE16 AD18:AE22 AD24:AE28">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF10 AF12:AF16 AF18:AF22 AF24:AF28">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X10 X12:X16 X18:X22 X24:X28">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN10 AN12:AN16 AN18:AN22 AN24:AN28">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO10">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO10 AO12:AO16 AO18:AO22 AO24:AO28">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ10">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ10 AQ12:AQ16 AQ18:AQ22 AQ24:AQ28">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V10"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI10">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V10 V12:V16 V18:V22 V24:V28"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI10 AG12:AI16 AG18:AI22 AG24:AI28">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ10 AJ12:AJ16 AJ18:AJ22 AJ24:AJ28">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK10 AK12:AK16 AK18:AK22 AK24:AK28">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -2416,13 +4467,13 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H10</xm:sqref>
+          <xm:sqref>H6:H10 H12:H16 H18:H22 H24:H28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I6:I10</xm:sqref>
+          <xm:sqref>I6:I10 I12:I16 I18:I22 I24:I28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2432,10 +4483,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2465,7 +4516,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -2488,7 +4539,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -2511,7 +4562,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -2534,7 +4585,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <v>50</v>
@@ -2557,7 +4608,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6">
         <v>60</v>
@@ -2575,6 +4626,351 @@
         <v>65</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>65</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>65</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>65</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>65</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>65</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>65</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>65</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <v>65</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>65</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>65</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
     </row>
@@ -2716,7 +5112,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2754,7 +5150,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>100</v>

</xml_diff>